<commit_message>
Remove obsolete binary files and update dashboard callbacks for improved project handling
- Deleted outdated binary files: `StringingCompiled_Output.xlsx`, `MicroPlanIndex.parquet`, `MicroPlanResponsibilities.parquet`, `ProdDailyExpandedSingles.parquet`, `ProjectBaselines.parquet`, `ProjectBaselinesMonthly.parquet`, `ProjectDetails.parquet`, `RawData.parquet`, and `StringingCompiled.parquet`.
- Updated `callbacks.py` to enhance project data handling, including improved PCH normalization and project display logic.
- Added logic to handle cases where Micro Plans are unavailable, ensuring robust project data representation.
</commit_message>
<xml_diff>
--- a/Raw Data/Micro Plans/Micro Plan - TB-408 Oct'25.xlsx
+++ b/Raw Data/Micro Plans/Micro Plan - TB-408 Oct'25.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaushikb\Documents\Work\Git\Office-work-\Test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaushikb\Documents\Work\Git\Office-work-\Raw Data\Micro Plans\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D577144C-B8E6-4A81-9CD7-46CDAA23ED27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A32D710A-A1C3-4DD9-85AB-20E53640C8B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="757" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1067,7 +1067,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="188">
+  <cellXfs count="187">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1498,9 +1498,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1528,15 +1525,60 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1552,51 +1594,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1612,9 +1609,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1622,6 +1616,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1662,6 +1659,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1672,6 +1689,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -1702,6 +1729,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -1712,6 +1749,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -1722,6 +1769,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -1732,6 +1799,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -1742,6 +1819,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1752,6 +1849,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -1782,6 +1889,46 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -1792,6 +1939,36 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -1812,6 +1989,56 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1822,6 +2049,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -1832,6 +2079,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -1842,6 +2099,36 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1862,6 +2149,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1882,6 +2179,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -1922,6 +2239,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -1932,6 +2269,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -1962,6 +2319,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -1972,6 +2339,36 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -2002,6 +2399,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -2032,6 +2439,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -2042,6 +2459,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -2062,6 +2489,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -2072,6 +2519,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -2082,6 +2549,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -2092,6 +2579,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -2102,6 +2599,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -2112,6 +2619,36 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -2132,6 +2669,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -2142,6 +2689,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -2152,6 +2719,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -2162,6 +2739,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -2192,6 +2789,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -2202,6 +2809,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -2212,6 +2829,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -2222,6 +2849,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -2242,6 +2879,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -2252,6 +2899,36 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -2272,6 +2949,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -2282,6 +2969,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -2292,6 +2989,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -2302,6 +3009,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -2322,6 +3039,96 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -2332,6 +3139,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -2342,6 +3159,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -2352,6 +3179,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -2362,6 +3199,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -2382,6 +3229,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -2392,6 +3249,46 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -2402,6 +3299,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -2412,6 +3329,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -2472,6 +3399,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -2482,951 +3419,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4574,137 +4571,137 @@
       <c r="F17" s="6"/>
     </row>
     <row r="18" spans="1:33" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="161" t="s">
+      <c r="A18" s="175" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="161" t="s">
+      <c r="B18" s="175" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="158" t="s">
+      <c r="C18" s="171" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="161" t="s">
+      <c r="D18" s="175" t="s">
         <v>7</v>
       </c>
-      <c r="E18" s="158" t="s">
+      <c r="E18" s="171" t="s">
         <v>16</v>
       </c>
-      <c r="F18" s="158" t="s">
+      <c r="F18" s="171" t="s">
         <v>17</v>
       </c>
-      <c r="G18" s="161" t="s">
+      <c r="G18" s="175" t="s">
         <v>8</v>
       </c>
-      <c r="H18" s="173" t="s">
+      <c r="H18" s="162" t="s">
         <v>18</v>
       </c>
-      <c r="I18" s="173"/>
-      <c r="J18" s="173"/>
-      <c r="K18" s="173"/>
-      <c r="L18" s="173"/>
-      <c r="M18" s="173"/>
-      <c r="N18" s="173"/>
-      <c r="O18" s="173"/>
-      <c r="P18" s="166" t="s">
+      <c r="I18" s="162"/>
+      <c r="J18" s="162"/>
+      <c r="K18" s="162"/>
+      <c r="L18" s="162"/>
+      <c r="M18" s="162"/>
+      <c r="N18" s="162"/>
+      <c r="O18" s="162"/>
+      <c r="P18" s="165" t="s">
         <v>19</v>
       </c>
-      <c r="R18" s="158" t="s">
+      <c r="R18" s="171" t="s">
         <v>36</v>
       </c>
-      <c r="T18" s="167" t="s">
+      <c r="T18" s="166" t="s">
         <v>31</v>
       </c>
-      <c r="U18" s="168"/>
-      <c r="V18" s="168"/>
-      <c r="W18" s="168"/>
-      <c r="X18" s="168"/>
-      <c r="Y18" s="169"/>
-      <c r="AA18" s="167" t="s">
+      <c r="U18" s="167"/>
+      <c r="V18" s="167"/>
+      <c r="W18" s="167"/>
+      <c r="X18" s="167"/>
+      <c r="Y18" s="168"/>
+      <c r="AA18" s="166" t="s">
         <v>30</v>
       </c>
-      <c r="AB18" s="168"/>
-      <c r="AC18" s="168"/>
-      <c r="AD18" s="168"/>
-      <c r="AE18" s="168"/>
-      <c r="AF18" s="169"/>
-      <c r="AG18" s="170" t="s">
+      <c r="AB18" s="167"/>
+      <c r="AC18" s="167"/>
+      <c r="AD18" s="167"/>
+      <c r="AE18" s="167"/>
+      <c r="AF18" s="168"/>
+      <c r="AG18" s="169" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:33" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="162"/>
-      <c r="B19" s="162"/>
-      <c r="C19" s="159"/>
-      <c r="D19" s="162"/>
-      <c r="E19" s="159"/>
-      <c r="F19" s="159"/>
-      <c r="G19" s="162"/>
-      <c r="H19" s="178" t="s">
+      <c r="A19" s="176"/>
+      <c r="B19" s="176"/>
+      <c r="C19" s="173"/>
+      <c r="D19" s="176"/>
+      <c r="E19" s="173"/>
+      <c r="F19" s="173"/>
+      <c r="G19" s="176"/>
+      <c r="H19" s="161" t="s">
         <v>9</v>
       </c>
-      <c r="I19" s="178"/>
-      <c r="J19" s="178" t="s">
+      <c r="I19" s="161"/>
+      <c r="J19" s="161" t="s">
         <v>12</v>
       </c>
-      <c r="K19" s="178"/>
-      <c r="L19" s="178" t="s">
+      <c r="K19" s="161"/>
+      <c r="L19" s="161" t="s">
         <v>13</v>
       </c>
-      <c r="M19" s="178"/>
-      <c r="N19" s="174" t="s">
+      <c r="M19" s="161"/>
+      <c r="N19" s="159" t="s">
         <v>15</v>
       </c>
-      <c r="O19" s="174" t="s">
+      <c r="O19" s="159" t="s">
         <v>14</v>
       </c>
-      <c r="P19" s="166"/>
+      <c r="P19" s="165"/>
       <c r="R19" s="172"/>
-      <c r="T19" s="164" t="s">
+      <c r="T19" s="163" t="s">
         <v>24</v>
       </c>
-      <c r="U19" s="164" t="s">
+      <c r="U19" s="163" t="s">
         <v>25</v>
       </c>
-      <c r="V19" s="164" t="s">
+      <c r="V19" s="163" t="s">
         <v>26</v>
       </c>
-      <c r="W19" s="164" t="s">
+      <c r="W19" s="163" t="s">
         <v>27</v>
       </c>
-      <c r="X19" s="164" t="s">
+      <c r="X19" s="163" t="s">
         <v>28</v>
       </c>
       <c r="Y19" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="AA19" s="164" t="s">
+      <c r="AA19" s="163" t="s">
         <v>24</v>
       </c>
-      <c r="AB19" s="164" t="s">
+      <c r="AB19" s="163" t="s">
         <v>25</v>
       </c>
-      <c r="AC19" s="164" t="s">
+      <c r="AC19" s="163" t="s">
         <v>26</v>
       </c>
-      <c r="AD19" s="164" t="s">
+      <c r="AD19" s="163" t="s">
         <v>27</v>
       </c>
-      <c r="AE19" s="164" t="s">
+      <c r="AE19" s="163" t="s">
         <v>28</v>
       </c>
       <c r="AF19" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="AG19" s="171"/>
+      <c r="AG19" s="170"/>
     </row>
     <row r="20" spans="1:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="163"/>
-      <c r="B20" s="162"/>
-      <c r="C20" s="159"/>
-      <c r="D20" s="162"/>
-      <c r="E20" s="160"/>
-      <c r="F20" s="160"/>
-      <c r="G20" s="162"/>
+      <c r="A20" s="177"/>
+      <c r="B20" s="176"/>
+      <c r="C20" s="173"/>
+      <c r="D20" s="176"/>
+      <c r="E20" s="174"/>
+      <c r="F20" s="174"/>
+      <c r="G20" s="176"/>
       <c r="H20" s="94" t="s">
         <v>10</v>
       </c>
@@ -4723,25 +4720,25 @@
       <c r="M20" s="94" t="s">
         <v>11</v>
       </c>
-      <c r="N20" s="175"/>
-      <c r="O20" s="175"/>
+      <c r="N20" s="160"/>
+      <c r="O20" s="160"/>
       <c r="P20" s="44" t="s">
         <v>51</v>
       </c>
       <c r="R20" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="T20" s="165"/>
-      <c r="U20" s="165"/>
-      <c r="V20" s="165"/>
-      <c r="W20" s="165"/>
-      <c r="X20" s="165"/>
+      <c r="T20" s="164"/>
+      <c r="U20" s="164"/>
+      <c r="V20" s="164"/>
+      <c r="W20" s="164"/>
+      <c r="X20" s="164"/>
       <c r="Y20" s="19"/>
-      <c r="AA20" s="165"/>
-      <c r="AB20" s="165"/>
-      <c r="AC20" s="165"/>
-      <c r="AD20" s="165"/>
-      <c r="AE20" s="165"/>
+      <c r="AA20" s="164"/>
+      <c r="AB20" s="164"/>
+      <c r="AC20" s="164"/>
+      <c r="AD20" s="164"/>
+      <c r="AE20" s="164"/>
       <c r="AF20" s="19" t="s">
         <v>51</v>
       </c>
@@ -5012,7 +5009,7 @@
       <c r="D25" s="86"/>
       <c r="E25" s="102"/>
       <c r="F25" s="8"/>
-      <c r="G25" s="176"/>
+      <c r="G25" s="157"/>
       <c r="H25" s="100"/>
       <c r="I25" s="100"/>
       <c r="J25" s="100"/>
@@ -5070,7 +5067,7 @@
       <c r="D26" s="8"/>
       <c r="E26" s="103"/>
       <c r="F26" s="97"/>
-      <c r="G26" s="177"/>
+      <c r="G26" s="158"/>
       <c r="H26" s="100"/>
       <c r="I26" s="100"/>
       <c r="J26" s="100"/>
@@ -5425,16 +5422,13 @@
     <filterColumn colId="13" showButton="0"/>
   </autoFilter>
   <mergeCells count="29">
-    <mergeCell ref="G25:G26"/>
-    <mergeCell ref="O19:O20"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="H18:O18"/>
-    <mergeCell ref="N19:N20"/>
-    <mergeCell ref="U19:U20"/>
-    <mergeCell ref="V19:V20"/>
-    <mergeCell ref="W19:W20"/>
+    <mergeCell ref="F18:F20"/>
+    <mergeCell ref="G18:G20"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="D18:D20"/>
+    <mergeCell ref="E18:E20"/>
     <mergeCell ref="X19:X20"/>
     <mergeCell ref="P18:P19"/>
     <mergeCell ref="AA18:AF18"/>
@@ -5447,13 +5441,16 @@
     <mergeCell ref="R18:R19"/>
     <mergeCell ref="T18:Y18"/>
     <mergeCell ref="T19:T20"/>
-    <mergeCell ref="F18:F20"/>
-    <mergeCell ref="G18:G20"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="D18:D20"/>
-    <mergeCell ref="E18:E20"/>
+    <mergeCell ref="H18:O18"/>
+    <mergeCell ref="N19:N20"/>
+    <mergeCell ref="U19:U20"/>
+    <mergeCell ref="V19:V20"/>
+    <mergeCell ref="W19:W20"/>
+    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="O19:O20"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="L19:M19"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B21">
@@ -5729,7 +5726,7 @@
       <c r="Q4" s="70">
         <v>0</v>
       </c>
-      <c r="R4" s="179" t="s">
+      <c r="R4" s="178" t="s">
         <v>76</v>
       </c>
     </row>
@@ -5772,14 +5769,14 @@
       <c r="Q5" s="70">
         <v>0</v>
       </c>
-      <c r="R5" s="180"/>
+      <c r="R5" s="179"/>
     </row>
     <row r="6" spans="2:18" s="75" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="181" t="s">
+      <c r="B6" s="180" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="182"/>
-      <c r="D6" s="183"/>
+      <c r="C6" s="181"/>
+      <c r="D6" s="182"/>
       <c r="E6" s="73">
         <v>160</v>
       </c>
@@ -5822,7 +5819,7 @@
   <dimension ref="A1:AK31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5886,25 +5883,25 @@
       <c r="I1" s="132" t="s">
         <v>112</v>
       </c>
-      <c r="J1" s="146" t="s">
+      <c r="J1" s="154" t="s">
         <v>120</v>
       </c>
-      <c r="K1" s="155" t="s">
+      <c r="K1" s="154" t="s">
         <v>117</v>
       </c>
-      <c r="L1" s="155" t="s">
+      <c r="L1" s="154" t="s">
         <v>118</v>
       </c>
-      <c r="M1" s="146" t="s">
+      <c r="M1" s="154" t="s">
         <v>38</v>
       </c>
-      <c r="N1" s="146" t="s">
+      <c r="N1" s="154" t="s">
         <v>39</v>
       </c>
       <c r="O1" s="156" t="s">
         <v>116</v>
       </c>
-      <c r="P1" s="157" t="s">
+      <c r="P1" s="155" t="s">
         <v>121</v>
       </c>
     </row>
@@ -5912,19 +5909,19 @@
       <c r="A2" s="8">
         <v>1</v>
       </c>
-      <c r="B2" s="148" t="s">
+      <c r="B2" s="147" t="s">
         <v>122</v>
       </c>
       <c r="C2" s="99" t="s">
         <v>50</v>
       </c>
-      <c r="D2" s="153">
+      <c r="D2" s="152">
         <v>37.504372000000004</v>
       </c>
       <c r="E2" s="120" t="s">
         <v>158</v>
       </c>
-      <c r="F2" s="147">
+      <c r="F2" s="146">
         <v>30</v>
       </c>
       <c r="G2" s="120" t="s">
@@ -5954,7 +5951,7 @@
         <f>+L2+1</f>
         <v>45934</v>
       </c>
-      <c r="O2" s="154">
+      <c r="O2" s="153">
         <f>+D2*8831</f>
         <v>331201.10913200001</v>
       </c>
@@ -5964,13 +5961,13 @@
       <c r="A3" s="8">
         <v>2</v>
       </c>
-      <c r="B3" s="148" t="s">
+      <c r="B3" s="147" t="s">
         <v>123</v>
       </c>
       <c r="C3" s="99" t="s">
         <v>80</v>
       </c>
-      <c r="D3" s="153">
+      <c r="D3" s="152">
         <v>45.413028000000004</v>
       </c>
       <c r="E3" s="120" t="s">
@@ -6007,7 +6004,7 @@
         <f t="shared" ref="N3:N30" si="2">+L3+1</f>
         <v>45943</v>
       </c>
-      <c r="O3" s="154">
+      <c r="O3" s="153">
         <f t="shared" ref="O3:O30" si="3">+D3*8831</f>
         <v>401042.45026800002</v>
       </c>
@@ -6033,13 +6030,13 @@
       <c r="A4" s="8">
         <v>3</v>
       </c>
-      <c r="B4" s="148" t="s">
+      <c r="B4" s="147" t="s">
         <v>124</v>
       </c>
       <c r="C4" s="99" t="s">
         <v>149</v>
       </c>
-      <c r="D4" s="153">
+      <c r="D4" s="152">
         <v>38.847605999999992</v>
       </c>
       <c r="E4" s="120" t="s">
@@ -6075,7 +6072,7 @@
         <f t="shared" si="2"/>
         <v>45949</v>
       </c>
-      <c r="O4" s="154">
+      <c r="O4" s="153">
         <f t="shared" si="3"/>
         <v>343063.20858599991</v>
       </c>
@@ -6101,13 +6098,13 @@
       <c r="A5" s="8">
         <v>4</v>
       </c>
-      <c r="B5" s="148" t="s">
+      <c r="B5" s="147" t="s">
         <v>125</v>
       </c>
       <c r="C5" s="99" t="s">
         <v>149</v>
       </c>
-      <c r="D5" s="153">
+      <c r="D5" s="152">
         <v>38.847605999999992</v>
       </c>
       <c r="E5" s="120" t="s">
@@ -6143,7 +6140,7 @@
         <f t="shared" si="2"/>
         <v>45955</v>
       </c>
-      <c r="O5" s="154">
+      <c r="O5" s="153">
         <f t="shared" si="3"/>
         <v>343063.20858599991</v>
       </c>
@@ -6169,13 +6166,13 @@
       <c r="A6" s="8">
         <v>5</v>
       </c>
-      <c r="B6" s="148" t="s">
+      <c r="B6" s="147" t="s">
         <v>126</v>
       </c>
       <c r="C6" s="99" t="s">
         <v>150</v>
       </c>
-      <c r="D6" s="153">
+      <c r="D6" s="152">
         <v>60.096777000000003</v>
       </c>
       <c r="E6" s="120" t="s">
@@ -6211,7 +6208,7 @@
         <f t="shared" si="2"/>
         <v>45961</v>
       </c>
-      <c r="O6" s="154">
+      <c r="O6" s="153">
         <f t="shared" si="3"/>
         <v>530714.63768699998</v>
       </c>
@@ -6237,13 +6234,13 @@
       <c r="A7" s="8">
         <v>6</v>
       </c>
-      <c r="B7" s="148" t="s">
+      <c r="B7" s="147" t="s">
         <v>127</v>
       </c>
       <c r="C7" s="99" t="s">
         <v>50</v>
       </c>
-      <c r="D7" s="153">
+      <c r="D7" s="152">
         <v>37.5</v>
       </c>
       <c r="E7" s="133" t="s">
@@ -6280,7 +6277,7 @@
         <f t="shared" si="2"/>
         <v>45941</v>
       </c>
-      <c r="O7" s="154">
+      <c r="O7" s="153">
         <f t="shared" si="3"/>
         <v>331162.5</v>
       </c>
@@ -6306,13 +6303,13 @@
       <c r="A8" s="8">
         <v>7</v>
       </c>
-      <c r="B8" s="149" t="s">
+      <c r="B8" s="148" t="s">
         <v>128</v>
       </c>
       <c r="C8" s="99" t="s">
         <v>151</v>
       </c>
-      <c r="D8" s="153">
+      <c r="D8" s="152">
         <v>67.873650999999995</v>
       </c>
       <c r="E8" s="133" t="s">
@@ -6347,7 +6344,7 @@
         <f t="shared" si="2"/>
         <v>45943</v>
       </c>
-      <c r="O8" s="154">
+      <c r="O8" s="153">
         <f t="shared" si="3"/>
         <v>599392.21198099991</v>
       </c>
@@ -6373,13 +6370,13 @@
       <c r="A9" s="8">
         <v>8</v>
       </c>
-      <c r="B9" s="149" t="s">
+      <c r="B9" s="148" t="s">
         <v>129</v>
       </c>
       <c r="C9" s="99" t="s">
         <v>88</v>
       </c>
-      <c r="D9" s="153">
+      <c r="D9" s="152">
         <v>47.184350000000002</v>
       </c>
       <c r="E9" s="133" t="s">
@@ -6415,7 +6412,7 @@
         <f t="shared" si="2"/>
         <v>45949</v>
       </c>
-      <c r="O9" s="154">
+      <c r="O9" s="153">
         <f t="shared" si="3"/>
         <v>416684.99485000002</v>
       </c>
@@ -6441,13 +6438,13 @@
       <c r="A10" s="8">
         <v>9</v>
       </c>
-      <c r="B10" s="149" t="s">
+      <c r="B10" s="148" t="s">
         <v>130</v>
       </c>
       <c r="C10" s="99" t="s">
         <v>152</v>
       </c>
-      <c r="D10" s="153">
+      <c r="D10" s="152">
         <v>57.597240999999997</v>
       </c>
       <c r="E10" s="120" t="s">
@@ -6485,7 +6482,7 @@
         <f t="shared" si="2"/>
         <v>45955</v>
       </c>
-      <c r="O10" s="154">
+      <c r="O10" s="153">
         <f t="shared" si="3"/>
         <v>508641.23527099995</v>
       </c>
@@ -6511,13 +6508,13 @@
       <c r="A11" s="8">
         <v>10</v>
       </c>
-      <c r="B11" s="149" t="s">
+      <c r="B11" s="148" t="s">
         <v>131</v>
       </c>
       <c r="C11" s="99" t="s">
         <v>153</v>
       </c>
-      <c r="D11" s="153">
+      <c r="D11" s="152">
         <v>67.873650999999995</v>
       </c>
       <c r="E11" s="120" t="s">
@@ -6553,7 +6550,7 @@
         <f t="shared" si="2"/>
         <v>45961</v>
       </c>
-      <c r="O11" s="154">
+      <c r="O11" s="153">
         <f t="shared" si="3"/>
         <v>599392.21198099991</v>
       </c>
@@ -6579,13 +6576,13 @@
       <c r="A12" s="8">
         <v>11</v>
       </c>
-      <c r="B12" s="150" t="s">
+      <c r="B12" s="149" t="s">
         <v>132</v>
       </c>
       <c r="C12" s="99" t="s">
         <v>50</v>
       </c>
-      <c r="D12" s="153">
+      <c r="D12" s="152">
         <v>37.504372000000004</v>
       </c>
       <c r="E12" s="120" t="s">
@@ -6620,7 +6617,7 @@
         <f t="shared" si="2"/>
         <v>45948</v>
       </c>
-      <c r="O12" s="154">
+      <c r="O12" s="153">
         <f t="shared" si="3"/>
         <v>331201.10913200001</v>
       </c>
@@ -6646,13 +6643,13 @@
       <c r="A13" s="8">
         <v>12</v>
       </c>
-      <c r="B13" s="148" t="s">
+      <c r="B13" s="147" t="s">
         <v>133</v>
       </c>
       <c r="C13" s="99" t="s">
         <v>50</v>
       </c>
-      <c r="D13" s="153">
+      <c r="D13" s="152">
         <v>37.504372000000004</v>
       </c>
       <c r="E13" s="120" t="s">
@@ -6686,7 +6683,7 @@
         <f t="shared" si="2"/>
         <v>45937</v>
       </c>
-      <c r="O13" s="154">
+      <c r="O13" s="153">
         <f t="shared" si="3"/>
         <v>331201.10913200001</v>
       </c>
@@ -6712,13 +6709,13 @@
       <c r="A14" s="8">
         <v>13</v>
       </c>
-      <c r="B14" s="148" t="s">
+      <c r="B14" s="147" t="s">
         <v>134</v>
       </c>
       <c r="C14" s="99" t="s">
         <v>154</v>
       </c>
-      <c r="D14" s="153">
+      <c r="D14" s="152">
         <v>66.381106999999986</v>
       </c>
       <c r="E14" s="120" t="s">
@@ -6755,7 +6752,7 @@
         <f t="shared" si="2"/>
         <v>45940</v>
       </c>
-      <c r="O14" s="154">
+      <c r="O14" s="153">
         <f t="shared" si="3"/>
         <v>586211.55591699993</v>
       </c>
@@ -6782,13 +6779,13 @@
       <c r="A15" s="8">
         <v>14</v>
       </c>
-      <c r="B15" s="148" t="s">
+      <c r="B15" s="147" t="s">
         <v>135</v>
       </c>
       <c r="C15" s="99" t="s">
         <v>80</v>
       </c>
-      <c r="D15" s="153">
+      <c r="D15" s="152">
         <v>45.413028000000004</v>
       </c>
       <c r="E15" s="120" t="s">
@@ -6824,7 +6821,7 @@
         <f t="shared" si="2"/>
         <v>45945</v>
       </c>
-      <c r="O15" s="154">
+      <c r="O15" s="153">
         <f t="shared" si="3"/>
         <v>401042.45026800002</v>
       </c>
@@ -6850,13 +6847,13 @@
       <c r="A16" s="8">
         <v>15</v>
       </c>
-      <c r="B16" s="148" t="s">
+      <c r="B16" s="147" t="s">
         <v>136</v>
       </c>
       <c r="C16" s="125" t="s">
         <v>155</v>
       </c>
-      <c r="D16" s="152">
+      <c r="D16" s="151">
         <v>78.132046999999986</v>
       </c>
       <c r="E16" s="120" t="s">
@@ -6891,7 +6888,7 @@
         <f t="shared" si="2"/>
         <v>45950</v>
       </c>
-      <c r="O16" s="154">
+      <c r="O16" s="153">
         <f t="shared" si="3"/>
         <v>689984.10705699993</v>
       </c>
@@ -6917,13 +6914,13 @@
       <c r="A17" s="8">
         <v>16</v>
       </c>
-      <c r="B17" s="151" t="s">
+      <c r="B17" s="150" t="s">
         <v>137</v>
       </c>
       <c r="C17" s="99" t="s">
         <v>50</v>
       </c>
-      <c r="D17" s="153">
+      <c r="D17" s="152">
         <v>37.504372000000004</v>
       </c>
       <c r="E17" s="120" t="s">
@@ -6959,7 +6956,7 @@
         <f t="shared" si="2"/>
         <v>45956</v>
       </c>
-      <c r="O17" s="154">
+      <c r="O17" s="153">
         <f t="shared" si="3"/>
         <v>331201.10913200001</v>
       </c>
@@ -6985,13 +6982,13 @@
       <c r="A18" s="8">
         <v>17</v>
       </c>
-      <c r="B18" s="148" t="s">
+      <c r="B18" s="147" t="s">
         <v>138</v>
       </c>
       <c r="C18" s="99" t="s">
         <v>156</v>
       </c>
-      <c r="D18" s="152">
+      <c r="D18" s="151">
         <v>66.381106999999986</v>
       </c>
       <c r="E18" s="120" t="s">
@@ -7026,7 +7023,7 @@
         <f t="shared" si="2"/>
         <v>45962</v>
       </c>
-      <c r="O18" s="154">
+      <c r="O18" s="153">
         <f t="shared" si="3"/>
         <v>586211.55591699993</v>
       </c>
@@ -7052,13 +7049,13 @@
       <c r="A19" s="8">
         <v>18</v>
       </c>
-      <c r="B19" s="148" t="s">
+      <c r="B19" s="147" t="s">
         <v>139</v>
       </c>
       <c r="C19" s="99" t="s">
         <v>80</v>
       </c>
-      <c r="D19" s="153">
+      <c r="D19" s="152">
         <v>45.413028000000004</v>
       </c>
       <c r="E19" s="133" t="s">
@@ -7095,7 +7092,7 @@
         <f t="shared" si="2"/>
         <v>45942</v>
       </c>
-      <c r="O19" s="154">
+      <c r="O19" s="153">
         <f t="shared" si="3"/>
         <v>401042.45026800002</v>
       </c>
@@ -7121,13 +7118,13 @@
       <c r="A20" s="8">
         <v>19</v>
       </c>
-      <c r="B20" s="148" t="s">
+      <c r="B20" s="147" t="s">
         <v>140</v>
       </c>
       <c r="C20" s="99" t="s">
         <v>80</v>
       </c>
-      <c r="D20" s="153">
+      <c r="D20" s="152">
         <v>45.413028000000004</v>
       </c>
       <c r="E20" s="133" t="s">
@@ -7163,7 +7160,7 @@
         <f t="shared" si="2"/>
         <v>45947</v>
       </c>
-      <c r="O20" s="154">
+      <c r="O20" s="153">
         <f t="shared" si="3"/>
         <v>401042.45026800002</v>
       </c>
@@ -7189,13 +7186,13 @@
       <c r="A21" s="8">
         <v>20</v>
       </c>
-      <c r="B21" s="151" t="s">
+      <c r="B21" s="150" t="s">
         <v>141</v>
       </c>
       <c r="C21" s="99" t="s">
         <v>50</v>
       </c>
-      <c r="D21" s="153">
+      <c r="D21" s="152">
         <v>37.504372000000004</v>
       </c>
       <c r="E21" s="133" t="s">
@@ -7231,7 +7228,7 @@
         <f t="shared" si="2"/>
         <v>45952</v>
       </c>
-      <c r="O21" s="154">
+      <c r="O21" s="153">
         <f t="shared" si="3"/>
         <v>331201.10913200001</v>
       </c>
@@ -7257,13 +7254,13 @@
       <c r="A22" s="8">
         <v>21</v>
       </c>
-      <c r="B22" s="148" t="s">
+      <c r="B22" s="147" t="s">
         <v>142</v>
       </c>
       <c r="C22" s="99" t="s">
         <v>50</v>
       </c>
-      <c r="D22" s="153">
+      <c r="D22" s="152">
         <v>37.504372000000004</v>
       </c>
       <c r="E22" s="133" t="s">
@@ -7299,7 +7296,7 @@
         <f t="shared" si="2"/>
         <v>45957</v>
       </c>
-      <c r="O22" s="154">
+      <c r="O22" s="153">
         <f t="shared" si="3"/>
         <v>331201.10913200001</v>
       </c>
@@ -7325,13 +7322,13 @@
       <c r="A23" s="8">
         <v>22</v>
       </c>
-      <c r="B23" s="148" t="s">
+      <c r="B23" s="147" t="s">
         <v>143</v>
       </c>
       <c r="C23" s="99" t="s">
         <v>88</v>
       </c>
-      <c r="D23" s="153">
+      <c r="D23" s="152">
         <v>47.184350000000002</v>
       </c>
       <c r="E23" s="133" t="s">
@@ -7367,7 +7364,7 @@
         <f t="shared" si="2"/>
         <v>45962</v>
       </c>
-      <c r="O23" s="154">
+      <c r="O23" s="153">
         <f t="shared" si="3"/>
         <v>416684.99485000002</v>
       </c>
@@ -7393,13 +7390,13 @@
       <c r="A24" s="8">
         <v>23</v>
       </c>
-      <c r="B24" s="148" t="s">
+      <c r="B24" s="147" t="s">
         <v>144</v>
       </c>
       <c r="C24" s="99" t="s">
         <v>50</v>
       </c>
-      <c r="D24" s="153">
+      <c r="D24" s="152">
         <v>37.504372000000004</v>
       </c>
       <c r="E24" s="133" t="s">
@@ -7433,7 +7430,7 @@
         <f t="shared" si="2"/>
         <v>45938</v>
       </c>
-      <c r="O24" s="154">
+      <c r="O24" s="153">
         <f t="shared" si="3"/>
         <v>331201.10913200001</v>
       </c>
@@ -7458,13 +7455,13 @@
       <c r="A25" s="8">
         <v>24</v>
       </c>
-      <c r="B25" s="148" t="s">
+      <c r="B25" s="147" t="s">
         <v>145</v>
       </c>
       <c r="C25" s="99" t="s">
         <v>50</v>
       </c>
-      <c r="D25" s="152">
+      <c r="D25" s="151">
         <v>37.504372000000004</v>
       </c>
       <c r="E25" s="133" t="s">
@@ -7502,7 +7499,7 @@
         <f t="shared" si="2"/>
         <v>45944</v>
       </c>
-      <c r="O25" s="154">
+      <c r="O25" s="153">
         <f t="shared" si="3"/>
         <v>331201.10913200001</v>
       </c>
@@ -7528,13 +7525,13 @@
       <c r="A26" s="8">
         <v>25</v>
       </c>
-      <c r="B26" s="148" t="s">
+      <c r="B26" s="147" t="s">
         <v>146</v>
       </c>
       <c r="C26" s="99" t="s">
         <v>149</v>
       </c>
-      <c r="D26" s="153">
+      <c r="D26" s="152">
         <v>38.847605999999992</v>
       </c>
       <c r="E26" s="133" t="s">
@@ -7570,7 +7567,7 @@
         <f t="shared" si="2"/>
         <v>45950</v>
       </c>
-      <c r="O26" s="154">
+      <c r="O26" s="153">
         <f t="shared" si="3"/>
         <v>343063.20858599991</v>
       </c>
@@ -7596,13 +7593,13 @@
       <c r="A27" s="8">
         <v>26</v>
       </c>
-      <c r="B27" s="148" t="s">
+      <c r="B27" s="147" t="s">
         <v>147</v>
       </c>
       <c r="C27" s="99" t="s">
         <v>157</v>
       </c>
-      <c r="D27" s="153">
+      <c r="D27" s="152">
         <v>89.1</v>
       </c>
       <c r="E27" s="133" t="s">
@@ -7638,7 +7635,7 @@
         <f t="shared" si="2"/>
         <v>45956</v>
       </c>
-      <c r="O27" s="154">
+      <c r="O27" s="153">
         <f t="shared" si="3"/>
         <v>786842.1</v>
       </c>
@@ -7664,13 +7661,13 @@
       <c r="A28" s="8">
         <v>27</v>
       </c>
-      <c r="B28" s="148" t="s">
+      <c r="B28" s="147" t="s">
         <v>92</v>
       </c>
       <c r="C28" s="99" t="s">
         <v>89</v>
       </c>
-      <c r="D28" s="153">
+      <c r="D28" s="152">
         <v>143.60187300000001</v>
       </c>
       <c r="E28" s="133" t="s">
@@ -7705,7 +7702,7 @@
         <f t="shared" si="2"/>
         <v>45940</v>
       </c>
-      <c r="O28" s="154">
+      <c r="O28" s="153">
         <f>+D28*9818</f>
         <v>1409883.1891140002</v>
       </c>
@@ -7731,13 +7728,13 @@
       <c r="A29" s="8">
         <v>28</v>
       </c>
-      <c r="B29" s="148" t="s">
+      <c r="B29" s="147" t="s">
         <v>93</v>
       </c>
       <c r="C29" s="99" t="s">
         <v>153</v>
       </c>
-      <c r="D29" s="153">
+      <c r="D29" s="152">
         <v>67.873650999999995</v>
       </c>
       <c r="E29" s="133" t="s">
@@ -7774,7 +7771,7 @@
         <f t="shared" si="2"/>
         <v>45941</v>
       </c>
-      <c r="O29" s="154">
+      <c r="O29" s="153">
         <f t="shared" si="3"/>
         <v>599392.21198099991</v>
       </c>
@@ -7800,13 +7797,13 @@
       <c r="A30" s="8">
         <v>29</v>
       </c>
-      <c r="B30" s="148" t="s">
+      <c r="B30" s="147" t="s">
         <v>148</v>
       </c>
       <c r="C30" s="99" t="s">
         <v>50</v>
       </c>
-      <c r="D30" s="153">
+      <c r="D30" s="152">
         <v>37.504372000000004</v>
       </c>
       <c r="E30" s="120" t="s">
@@ -7842,7 +7839,7 @@
         <f t="shared" si="2"/>
         <v>45952</v>
       </c>
-      <c r="O30" s="154">
+      <c r="O30" s="153">
         <f t="shared" si="3"/>
         <v>331201.10913200001</v>
       </c>
@@ -7879,8 +7876,8 @@
     <cfRule type="duplicateValues" dxfId="181" priority="33"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:B15">
-    <cfRule type="duplicateValues" dxfId="180" priority="34"/>
-    <cfRule type="duplicateValues" dxfId="179" priority="35"/>
+    <cfRule type="duplicateValues" dxfId="180" priority="35"/>
+    <cfRule type="duplicateValues" dxfId="179" priority="34"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:B30 B2:B11">
     <cfRule type="duplicateValues" dxfId="178" priority="36"/>
@@ -7900,14 +7897,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J30">
-    <cfRule type="containsText" dxfId="177" priority="63" operator="containsText" text="WIP">
-      <formula>NOT(ISERROR(SEARCH("WIP",J2)))</formula>
+    <cfRule type="containsText" dxfId="177" priority="70" operator="containsText" text="ROW">
+      <formula>NOT(ISERROR(SEARCH("ROW",J2)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="176" priority="69" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",J2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="175" priority="70" operator="containsText" text="ROW">
-      <formula>NOT(ISERROR(SEARCH("ROW",J2)))</formula>
+    <cfRule type="containsText" dxfId="175" priority="63" operator="containsText" text="WIP">
+      <formula>NOT(ISERROR(SEARCH("WIP",J2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:J15">
@@ -7924,28 +7921,28 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J10">
-    <cfRule type="containsText" dxfId="171" priority="198" operator="containsText" text="WIP">
-      <formula>NOT(ISERROR(SEARCH("WIP",J10)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="170" priority="199" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="171" priority="205" operator="containsText" text="ROW">
+      <formula>NOT(ISERROR(SEARCH("ROW",J10)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="170" priority="204" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",J10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="169" priority="200" operator="containsText" text="ROW">
+    <cfRule type="containsText" dxfId="169" priority="203" operator="containsText" text="ROW">
       <formula>NOT(ISERROR(SEARCH("ROW",J10)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="168" priority="202" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",J10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="167" priority="203" operator="containsText" text="ROW">
+    <cfRule type="containsText" dxfId="167" priority="201" operator="containsText" text="WIP">
+      <formula>NOT(ISERROR(SEARCH("WIP",J10)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="166" priority="200" operator="containsText" text="ROW">
       <formula>NOT(ISERROR(SEARCH("ROW",J10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="166" priority="204" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="165" priority="199" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",J10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="165" priority="205" operator="containsText" text="ROW">
-      <formula>NOT(ISERROR(SEARCH("ROW",J10)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="164" priority="201" operator="containsText" text="WIP">
+    <cfRule type="containsText" dxfId="164" priority="198" operator="containsText" text="WIP">
       <formula>NOT(ISERROR(SEARCH("WIP",J10)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7958,11 +7955,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J13:J14">
-    <cfRule type="containsText" dxfId="161" priority="67" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="161" priority="68" operator="containsText" text="ROW">
+      <formula>NOT(ISERROR(SEARCH("ROW",J13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="160" priority="67" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",J13)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="160" priority="68" operator="containsText" text="ROW">
-      <formula>NOT(ISERROR(SEARCH("ROW",J13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J15:J16 K15:L18 L14:N14 K15:N15">
@@ -7997,36 +7994,36 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J22:J23">
-    <cfRule type="containsText" dxfId="152" priority="54" operator="containsText" text="Complete">
-      <formula>NOT(ISERROR(SEARCH("Complete",J22)))</formula>
+    <cfRule type="containsText" dxfId="152" priority="55" operator="containsText" text="ROW">
+      <formula>NOT(ISERROR(SEARCH("ROW",J22)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="151" priority="56" operator="containsText" text="WIP">
       <formula>NOT(ISERROR(SEARCH("WIP",J22)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="150" priority="53" operator="containsText" text="WIP">
+    <cfRule type="containsText" dxfId="150" priority="54" operator="containsText" text="Complete">
+      <formula>NOT(ISERROR(SEARCH("Complete",J22)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="149" priority="53" operator="containsText" text="WIP">
       <formula>NOT(ISERROR(SEARCH("WIP",J22)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="149" priority="55" operator="containsText" text="ROW">
-      <formula>NOT(ISERROR(SEARCH("ROW",J22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J23:J30">
-    <cfRule type="containsText" dxfId="148" priority="43" operator="containsText" text="ROW">
-      <formula>NOT(ISERROR(SEARCH("ROW",J23)))</formula>
+    <cfRule type="containsText" dxfId="148" priority="41" operator="containsText" text="WIP">
+      <formula>NOT(ISERROR(SEARCH("WIP",J23)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="147" priority="42" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",J23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="146" priority="41" operator="containsText" text="WIP">
-      <formula>NOT(ISERROR(SEARCH("WIP",J23)))</formula>
+    <cfRule type="containsText" dxfId="146" priority="43" operator="containsText" text="ROW">
+      <formula>NOT(ISERROR(SEARCH("ROW",J23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J16:K16">
-    <cfRule type="containsText" dxfId="145" priority="247" operator="containsText" text="ROW">
+    <cfRule type="containsText" dxfId="145" priority="246" operator="containsText" text="Complete">
+      <formula>NOT(ISERROR(SEARCH("Complete",J16)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="144" priority="247" operator="containsText" text="ROW">
       <formula>NOT(ISERROR(SEARCH("ROW",J16)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="144" priority="246" operator="containsText" text="Complete">
-      <formula>NOT(ISERROR(SEARCH("Complete",J16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J18:K18">
@@ -8056,14 +8053,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:N4 K4:K6 L6:N6">
-    <cfRule type="containsText" dxfId="137" priority="260" operator="containsText" text="WIP">
-      <formula>NOT(ISERROR(SEARCH("WIP",J4)))</formula>
+    <cfRule type="containsText" dxfId="137" priority="262" operator="containsText" text="ROW">
+      <formula>NOT(ISERROR(SEARCH("ROW",J4)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="136" priority="261" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",J4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="135" priority="262" operator="containsText" text="ROW">
-      <formula>NOT(ISERROR(SEARCH("ROW",J4)))</formula>
+    <cfRule type="containsText" dxfId="135" priority="260" operator="containsText" text="WIP">
+      <formula>NOT(ISERROR(SEARCH("WIP",J4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J16:N16">
@@ -8078,28 +8075,28 @@
     <cfRule type="containsText" dxfId="132" priority="157" operator="containsText" text="WIP">
       <formula>NOT(ISERROR(SEARCH("WIP",J23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="131" priority="146" operator="containsText" text="WIP">
+    <cfRule type="containsText" dxfId="131" priority="150" operator="containsText" text="ROW">
+      <formula>NOT(ISERROR(SEARCH("ROW",J23)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="130" priority="149" operator="containsText" text="Complete">
+      <formula>NOT(ISERROR(SEARCH("Complete",J23)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="129" priority="147" operator="containsText" text="Complete">
+      <formula>NOT(ISERROR(SEARCH("Complete",J23)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="128" priority="146" operator="containsText" text="WIP">
       <formula>NOT(ISERROR(SEARCH("WIP",J23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="130" priority="147" operator="containsText" text="Complete">
-      <formula>NOT(ISERROR(SEARCH("Complete",J23)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="129" priority="148" operator="containsText" text="ROW">
-      <formula>NOT(ISERROR(SEARCH("ROW",J23)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="128" priority="149" operator="containsText" text="Complete">
-      <formula>NOT(ISERROR(SEARCH("Complete",J23)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="127" priority="150" operator="containsText" text="ROW">
+    <cfRule type="containsText" dxfId="127" priority="148" operator="containsText" text="ROW">
       <formula>NOT(ISERROR(SEARCH("ROW",J23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K6">
-    <cfRule type="containsText" dxfId="126" priority="234" operator="containsText" text="ROW">
+    <cfRule type="containsText" dxfId="126" priority="233" operator="containsText" text="Complete">
+      <formula>NOT(ISERROR(SEARCH("Complete",K2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="125" priority="234" operator="containsText" text="ROW">
       <formula>NOT(ISERROR(SEARCH("ROW",K2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="125" priority="233" operator="containsText" text="Complete">
-      <formula>NOT(ISERROR(SEARCH("Complete",K2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K28:K29 M28:N29">
@@ -8111,17 +8108,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K8:L11">
-    <cfRule type="containsText" dxfId="122" priority="21" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="122" priority="26" operator="containsText" text="ROW">
+      <formula>NOT(ISERROR(SEARCH("ROW",K8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="121" priority="25" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",K8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="121" priority="26" operator="containsText" text="ROW">
+    <cfRule type="containsText" dxfId="120" priority="22" operator="containsText" text="ROW">
       <formula>NOT(ISERROR(SEARCH("ROW",K8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="120" priority="25" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="119" priority="21" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",K8)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="119" priority="22" operator="containsText" text="ROW">
-      <formula>NOT(ISERROR(SEARCH("ROW",K8)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="118" priority="17" operator="containsText" text="WIP">
       <formula>NOT(ISERROR(SEARCH("WIP",K8)))</formula>
@@ -8147,14 +8144,14 @@
     <cfRule type="containsText" dxfId="113" priority="6" operator="containsText" text="ROW">
       <formula>NOT(ISERROR(SEARCH("ROW",K19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="112" priority="1" operator="containsText" text="WIP">
-      <formula>NOT(ISERROR(SEARCH("WIP",K19)))</formula>
+    <cfRule type="containsText" dxfId="112" priority="9" operator="containsText" text="Complete">
+      <formula>NOT(ISERROR(SEARCH("Complete",K19)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="111" priority="10" operator="containsText" text="ROW">
       <formula>NOT(ISERROR(SEARCH("ROW",K19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="110" priority="9" operator="containsText" text="Complete">
-      <formula>NOT(ISERROR(SEARCH("Complete",K19)))</formula>
+    <cfRule type="containsText" dxfId="110" priority="1" operator="containsText" text="WIP">
+      <formula>NOT(ISERROR(SEARCH("WIP",K19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K20:L23">
@@ -8169,14 +8166,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K21:L22">
-    <cfRule type="containsText" dxfId="106" priority="16" operator="containsText" text="ROW">
-      <formula>NOT(ISERROR(SEARCH("ROW",K21)))</formula>
+    <cfRule type="containsText" dxfId="106" priority="14" operator="containsText" text="WIP">
+      <formula>NOT(ISERROR(SEARCH("WIP",K21)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="105" priority="15" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",K21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="104" priority="14" operator="containsText" text="WIP">
-      <formula>NOT(ISERROR(SEARCH("WIP",K21)))</formula>
+    <cfRule type="containsText" dxfId="104" priority="16" operator="containsText" text="ROW">
+      <formula>NOT(ISERROR(SEARCH("ROW",K21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:N4 L3:L6 K4:K6">
@@ -8198,30 +8195,30 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5:N7 M8:N11 K10:L11 K12:N15 K15:L18">
-    <cfRule type="containsText" dxfId="99" priority="237" operator="containsText" text="ROW">
+    <cfRule type="containsText" dxfId="99" priority="236" operator="containsText" text="Complete">
+      <formula>NOT(ISERROR(SEARCH("Complete",K5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="98" priority="237" operator="containsText" text="ROW">
       <formula>NOT(ISERROR(SEARCH("ROW",K5)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="98" priority="236" operator="containsText" text="Complete">
-      <formula>NOT(ISERROR(SEARCH("Complete",K5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12:N12">
-    <cfRule type="containsText" dxfId="97" priority="79" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="97" priority="80" operator="containsText" text="ROW">
+      <formula>NOT(ISERROR(SEARCH("ROW",K12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="96" priority="79" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",K12)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="96" priority="80" operator="containsText" text="ROW">
-      <formula>NOT(ISERROR(SEARCH("ROW",K12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13:N14">
-    <cfRule type="containsText" dxfId="95" priority="218" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="95" priority="219" operator="containsText" text="ROW">
+      <formula>NOT(ISERROR(SEARCH("ROW",K13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="94" priority="218" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",K13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="94" priority="217" operator="containsText" text="WIP">
+    <cfRule type="containsText" dxfId="93" priority="217" operator="containsText" text="WIP">
       <formula>NOT(ISERROR(SEARCH("WIP",K13)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="93" priority="219" operator="containsText" text="ROW">
-      <formula>NOT(ISERROR(SEARCH("ROW",K13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K17:N18 M19:N20">
@@ -8240,14 +8237,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K23:N25 K25:L27">
-    <cfRule type="containsText" dxfId="89" priority="135" operator="containsText" text="WIP">
+    <cfRule type="containsText" dxfId="89" priority="136" operator="containsText" text="Complete">
+      <formula>NOT(ISERROR(SEARCH("Complete",K23)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="88" priority="137" operator="containsText" text="ROW">
+      <formula>NOT(ISERROR(SEARCH("ROW",K23)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="87" priority="135" operator="containsText" text="WIP">
       <formula>NOT(ISERROR(SEARCH("WIP",K23)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="88" priority="136" operator="containsText" text="Complete">
-      <formula>NOT(ISERROR(SEARCH("Complete",K23)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="87" priority="137" operator="containsText" text="ROW">
-      <formula>NOT(ISERROR(SEARCH("ROW",K23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K26:N27">
@@ -8262,14 +8259,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K30:N30">
-    <cfRule type="containsText" dxfId="83" priority="108" operator="containsText" text="WIP">
-      <formula>NOT(ISERROR(SEARCH("WIP",K30)))</formula>
+    <cfRule type="containsText" dxfId="83" priority="110" operator="containsText" text="ROW">
+      <formula>NOT(ISERROR(SEARCH("ROW",K30)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="82" priority="109" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",K30)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="81" priority="110" operator="containsText" text="ROW">
-      <formula>NOT(ISERROR(SEARCH("ROW",K30)))</formula>
+    <cfRule type="containsText" dxfId="81" priority="108" operator="containsText" text="WIP">
+      <formula>NOT(ISERROR(SEARCH("WIP",K30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L11">
@@ -8284,14 +8281,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L22">
-    <cfRule type="containsText" dxfId="77" priority="3" operator="containsText" text="Complete">
-      <formula>NOT(ISERROR(SEARCH("Complete",L22)))</formula>
+    <cfRule type="containsText" dxfId="77" priority="2" operator="containsText" text="WIP">
+      <formula>NOT(ISERROR(SEARCH("WIP",L22)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="76" priority="4" operator="containsText" text="ROW">
       <formula>NOT(ISERROR(SEARCH("ROW",L22)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="75" priority="2" operator="containsText" text="WIP">
-      <formula>NOT(ISERROR(SEARCH("WIP",L22)))</formula>
+    <cfRule type="containsText" dxfId="75" priority="3" operator="containsText" text="Complete">
+      <formula>NOT(ISERROR(SEARCH("Complete",L22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L25:L27 L25:N25">
@@ -8300,14 +8297,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L28:L29">
-    <cfRule type="containsText" dxfId="73" priority="30" operator="containsText" text="WIP">
-      <formula>NOT(ISERROR(SEARCH("WIP",L28)))</formula>
+    <cfRule type="containsText" dxfId="73" priority="32" operator="containsText" text="ROW">
+      <formula>NOT(ISERROR(SEARCH("ROW",L28)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="72" priority="31" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",L28)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="71" priority="32" operator="containsText" text="ROW">
-      <formula>NOT(ISERROR(SEARCH("ROW",L28)))</formula>
+    <cfRule type="containsText" dxfId="71" priority="30" operator="containsText" text="WIP">
+      <formula>NOT(ISERROR(SEARCH("WIP",L28)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:N2 M2:N30">
@@ -8324,18 +8321,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L6:N6">
-    <cfRule type="containsText" dxfId="67" priority="230" operator="containsText" text="WIP">
+    <cfRule type="containsText" dxfId="67" priority="232" operator="containsText" text="ROW">
+      <formula>NOT(ISERROR(SEARCH("ROW",L6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="66" priority="230" operator="containsText" text="WIP">
       <formula>NOT(ISERROR(SEARCH("WIP",L6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="231" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="65" priority="231" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",L6)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="65" priority="232" operator="containsText" text="ROW">
-      <formula>NOT(ISERROR(SEARCH("ROW",L6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L12:N12">
-    <cfRule type="containsText" dxfId="64" priority="83" operator="containsText" text="WIP">
+    <cfRule type="containsText" dxfId="64" priority="76" operator="containsText" text="WIP">
       <formula>NOT(ISERROR(SEARCH("WIP",L12)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="63" priority="84" operator="containsText" text="Complete">
@@ -8347,11 +8344,11 @@
     <cfRule type="containsText" dxfId="61" priority="77" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",L12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="76" operator="containsText" text="WIP">
+    <cfRule type="containsText" dxfId="60" priority="78" operator="containsText" text="ROW">
+      <formula>NOT(ISERROR(SEARCH("ROW",L12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="59" priority="83" operator="containsText" text="WIP">
       <formula>NOT(ISERROR(SEARCH("WIP",L12)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="59" priority="78" operator="containsText" text="ROW">
-      <formula>NOT(ISERROR(SEARCH("ROW",L12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L14:N14 J23:N23">
@@ -8363,14 +8360,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L14:N14">
-    <cfRule type="containsText" dxfId="56" priority="215" operator="containsText" text="Complete">
-      <formula>NOT(ISERROR(SEARCH("Complete",L14)))</formula>
+    <cfRule type="containsText" dxfId="56" priority="216" operator="containsText" text="ROW">
+      <formula>NOT(ISERROR(SEARCH("ROW",L14)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="55" priority="214" operator="containsText" text="WIP">
       <formula>NOT(ISERROR(SEARCH("WIP",L14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="216" operator="containsText" text="ROW">
-      <formula>NOT(ISERROR(SEARCH("ROW",L14)))</formula>
+    <cfRule type="containsText" dxfId="54" priority="215" operator="containsText" text="Complete">
+      <formula>NOT(ISERROR(SEARCH("Complete",L14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L14:N15 L15:L18">
@@ -8382,26 +8379,26 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L16:N16">
-    <cfRule type="containsText" dxfId="51" priority="192" operator="containsText" text="ROW">
+    <cfRule type="containsText" dxfId="51" priority="189" operator="containsText" text="ROW">
       <formula>NOT(ISERROR(SEARCH("ROW",L16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="191" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="50" priority="190" operator="containsText" text="WIP">
+      <formula>NOT(ISERROR(SEARCH("WIP",L16)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="49" priority="191" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",L16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="190" operator="containsText" text="WIP">
+    <cfRule type="containsText" dxfId="48" priority="192" operator="containsText" text="ROW">
+      <formula>NOT(ISERROR(SEARCH("ROW",L16)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="47" priority="195" operator="containsText" text="WIP">
       <formula>NOT(ISERROR(SEARCH("WIP",L16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="195" operator="containsText" text="WIP">
+    <cfRule type="containsText" dxfId="46" priority="188" operator="containsText" text="Complete">
+      <formula>NOT(ISERROR(SEARCH("Complete",L16)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="45" priority="187" operator="containsText" text="WIP">
       <formula>NOT(ISERROR(SEARCH("WIP",L16)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="47" priority="189" operator="containsText" text="ROW">
-      <formula>NOT(ISERROR(SEARCH("ROW",L16)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="187" operator="containsText" text="WIP">
-      <formula>NOT(ISERROR(SEARCH("WIP",L16)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="188" operator="containsText" text="Complete">
-      <formula>NOT(ISERROR(SEARCH("Complete",L16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L16:N18">
@@ -8424,37 +8421,37 @@
     <cfRule type="containsText" dxfId="40" priority="134" operator="containsText" text="ROW">
       <formula>NOT(ISERROR(SEARCH("ROW",L25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="133" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="39" priority="142" operator="containsText" text="ROW">
+      <formula>NOT(ISERROR(SEARCH("ROW",L25)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="38" priority="140" operator="containsText" text="WIP">
+      <formula>NOT(ISERROR(SEARCH("WIP",L25)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="37" priority="141" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",L25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="141" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="36" priority="133" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",L25)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="142" operator="containsText" text="ROW">
-      <formula>NOT(ISERROR(SEARCH("ROW",L25)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="140" operator="containsText" text="WIP">
-      <formula>NOT(ISERROR(SEARCH("WIP",L25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L27:N27">
-    <cfRule type="containsText" dxfId="35" priority="125" operator="containsText" text="ROW">
-      <formula>NOT(ISERROR(SEARCH("ROW",L27)))</formula>
+    <cfRule type="containsText" dxfId="35" priority="124" operator="containsText" text="Complete">
+      <formula>NOT(ISERROR(SEARCH("Complete",L27)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="34" priority="123" operator="containsText" text="WIP">
       <formula>NOT(ISERROR(SEARCH("WIP",L27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="131" operator="containsText" text="ROW">
+    <cfRule type="containsText" dxfId="33" priority="130" operator="containsText" text="Complete">
+      <formula>NOT(ISERROR(SEARCH("Complete",L27)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="32" priority="129" operator="containsText" text="WIP">
+      <formula>NOT(ISERROR(SEARCH("WIP",L27)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="31" priority="131" operator="containsText" text="ROW">
       <formula>NOT(ISERROR(SEARCH("ROW",L27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="130" operator="containsText" text="Complete">
-      <formula>NOT(ISERROR(SEARCH("Complete",L27)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="124" operator="containsText" text="Complete">
-      <formula>NOT(ISERROR(SEARCH("Complete",L27)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="129" operator="containsText" text="WIP">
-      <formula>NOT(ISERROR(SEARCH("WIP",L27)))</formula>
+    <cfRule type="containsText" dxfId="30" priority="125" operator="containsText" text="ROW">
+      <formula>NOT(ISERROR(SEARCH("ROW",L27)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:N30 L2:N2">
@@ -8480,14 +8477,14 @@
     <cfRule type="containsText" dxfId="24" priority="210" operator="containsText" text="ROW">
       <formula>NOT(ISERROR(SEARCH("ROW",M9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="211" operator="containsText" text="WIP">
-      <formula>NOT(ISERROR(SEARCH("WIP",M9)))</formula>
+    <cfRule type="containsText" dxfId="23" priority="213" operator="containsText" text="ROW">
+      <formula>NOT(ISERROR(SEARCH("ROW",M9)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="22" priority="212" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",M9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="213" operator="containsText" text="ROW">
-      <formula>NOT(ISERROR(SEARCH("ROW",M9)))</formula>
+    <cfRule type="containsText" dxfId="21" priority="211" operator="containsText" text="WIP">
+      <formula>NOT(ISERROR(SEARCH("WIP",M9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M19:N20 K17:N18">
@@ -8509,36 +8506,36 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M21:N21">
-    <cfRule type="containsText" dxfId="16" priority="163" operator="containsText" text="ROW">
+    <cfRule type="containsText" dxfId="16" priority="162" operator="containsText" text="Complete">
+      <formula>NOT(ISERROR(SEARCH("Complete",M21)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="15" priority="161" operator="containsText" text="WIP">
+      <formula>NOT(ISERROR(SEARCH("WIP",M21)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="14" priority="166" operator="containsText" text="WIP">
+      <formula>NOT(ISERROR(SEARCH("WIP",M21)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="163" operator="containsText" text="ROW">
       <formula>NOT(ISERROR(SEARCH("ROW",M21)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="162" operator="containsText" text="Complete">
-      <formula>NOT(ISERROR(SEARCH("Complete",M21)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="161" operator="containsText" text="WIP">
-      <formula>NOT(ISERROR(SEARCH("WIP",M21)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="166" operator="containsText" text="WIP">
-      <formula>NOT(ISERROR(SEARCH("WIP",M21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M21:N22 K23:N23">
     <cfRule type="containsText" dxfId="12" priority="156" operator="containsText" text="ROW">
       <formula>NOT(ISERROR(SEARCH("ROW",K21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="155" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="11" priority="154" operator="containsText" text="WIP">
+      <formula>NOT(ISERROR(SEARCH("WIP",K21)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="155" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",K21)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="154" operator="containsText" text="WIP">
-      <formula>NOT(ISERROR(SEARCH("WIP",K21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M22:N22 K23:N23">
-    <cfRule type="containsText" dxfId="9" priority="153" operator="containsText" text="ROW">
+    <cfRule type="containsText" dxfId="9" priority="152" operator="containsText" text="Complete">
+      <formula>NOT(ISERROR(SEARCH("Complete",K22)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="153" operator="containsText" text="ROW">
       <formula>NOT(ISERROR(SEARCH("ROW",K22)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="152" operator="containsText" text="Complete">
-      <formula>NOT(ISERROR(SEARCH("Complete",K22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M28:N29 K28:K29">
@@ -8547,10 +8544,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M29:N29">
-    <cfRule type="containsText" dxfId="6" priority="114" operator="containsText" text="WIP">
-      <formula>NOT(ISERROR(SEARCH("WIP",M29)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="115" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="6" priority="122" operator="containsText" text="ROW">
+      <formula>NOT(ISERROR(SEARCH("ROW",M29)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="121" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",M29)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="4" priority="120" operator="containsText" text="WIP">
@@ -8559,11 +8556,11 @@
     <cfRule type="containsText" dxfId="3" priority="116" operator="containsText" text="ROW">
       <formula>NOT(ISERROR(SEARCH("ROW",M29)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="121" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="2" priority="115" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",M29)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="122" operator="containsText" text="ROW">
-      <formula>NOT(ISERROR(SEARCH("ROW",M29)))</formula>
+    <cfRule type="containsText" dxfId="1" priority="114" operator="containsText" text="WIP">
+      <formula>NOT(ISERROR(SEARCH("WIP",M29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions horizontalCentered="1"/>
@@ -8865,118 +8862,118 @@
       <c r="F17" s="6"/>
     </row>
     <row r="18" spans="1:28" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="161" t="s">
+      <c r="A18" s="175" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="161" t="s">
+      <c r="B18" s="175" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="158" t="s">
+      <c r="C18" s="171" t="s">
         <v>47</v>
       </c>
-      <c r="D18" s="158" t="s">
+      <c r="D18" s="171" t="s">
         <v>43</v>
       </c>
-      <c r="E18" s="161" t="s">
+      <c r="E18" s="175" t="s">
         <v>8</v>
       </c>
-      <c r="F18" s="173" t="s">
+      <c r="F18" s="162" t="s">
         <v>18</v>
       </c>
-      <c r="G18" s="173"/>
-      <c r="H18" s="173"/>
-      <c r="I18" s="173"/>
-      <c r="J18" s="173"/>
-      <c r="K18" s="166" t="s">
+      <c r="G18" s="162"/>
+      <c r="H18" s="162"/>
+      <c r="I18" s="162"/>
+      <c r="J18" s="162"/>
+      <c r="K18" s="165" t="s">
         <v>19</v>
       </c>
-      <c r="M18" s="158" t="s">
+      <c r="M18" s="171" t="s">
         <v>36</v>
       </c>
-      <c r="O18" s="167" t="s">
+      <c r="O18" s="166" t="s">
         <v>31</v>
       </c>
-      <c r="P18" s="168"/>
-      <c r="Q18" s="168"/>
-      <c r="R18" s="168"/>
-      <c r="S18" s="168"/>
-      <c r="T18" s="169"/>
-      <c r="V18" s="167" t="s">
+      <c r="P18" s="167"/>
+      <c r="Q18" s="167"/>
+      <c r="R18" s="167"/>
+      <c r="S18" s="167"/>
+      <c r="T18" s="168"/>
+      <c r="V18" s="166" t="s">
         <v>30</v>
       </c>
-      <c r="W18" s="168"/>
-      <c r="X18" s="168"/>
-      <c r="Y18" s="168"/>
-      <c r="Z18" s="168"/>
-      <c r="AA18" s="169"/>
-      <c r="AB18" s="170" t="s">
+      <c r="W18" s="167"/>
+      <c r="X18" s="167"/>
+      <c r="Y18" s="167"/>
+      <c r="Z18" s="167"/>
+      <c r="AA18" s="168"/>
+      <c r="AB18" s="169" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="162"/>
-      <c r="B19" s="162"/>
-      <c r="C19" s="159"/>
-      <c r="D19" s="162"/>
-      <c r="E19" s="162"/>
-      <c r="F19" s="185" t="s">
+      <c r="A19" s="176"/>
+      <c r="B19" s="176"/>
+      <c r="C19" s="173"/>
+      <c r="D19" s="176"/>
+      <c r="E19" s="176"/>
+      <c r="F19" s="183" t="s">
         <v>40</v>
       </c>
-      <c r="G19" s="186" t="s">
+      <c r="G19" s="184" t="s">
         <v>44</v>
       </c>
-      <c r="H19" s="187"/>
-      <c r="I19" s="186" t="s">
+      <c r="H19" s="185"/>
+      <c r="I19" s="184" t="s">
         <v>45</v>
       </c>
-      <c r="J19" s="187"/>
-      <c r="K19" s="166"/>
+      <c r="J19" s="185"/>
+      <c r="K19" s="165"/>
       <c r="M19" s="172"/>
-      <c r="O19" s="164" t="s">
+      <c r="O19" s="163" t="s">
         <v>24</v>
       </c>
-      <c r="P19" s="164" t="s">
+      <c r="P19" s="163" t="s">
         <v>25</v>
       </c>
-      <c r="Q19" s="164" t="s">
+      <c r="Q19" s="163" t="s">
         <v>26</v>
       </c>
-      <c r="R19" s="164" t="s">
+      <c r="R19" s="163" t="s">
         <v>27</v>
       </c>
-      <c r="S19" s="164" t="s">
+      <c r="S19" s="163" t="s">
         <v>28</v>
       </c>
       <c r="T19" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="V19" s="164" t="s">
+      <c r="V19" s="163" t="s">
         <v>24</v>
       </c>
-      <c r="W19" s="164" t="s">
+      <c r="W19" s="163" t="s">
         <v>25</v>
       </c>
-      <c r="X19" s="164" t="s">
+      <c r="X19" s="163" t="s">
         <v>26</v>
       </c>
-      <c r="Y19" s="164" t="s">
+      <c r="Y19" s="163" t="s">
         <v>27</v>
       </c>
-      <c r="Z19" s="164" t="s">
+      <c r="Z19" s="163" t="s">
         <v>28</v>
       </c>
       <c r="AA19" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="AB19" s="171"/>
+      <c r="AB19" s="170"/>
     </row>
     <row r="20" spans="1:28" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="162"/>
-      <c r="B20" s="162"/>
-      <c r="C20" s="159"/>
-      <c r="D20" s="162"/>
-      <c r="E20" s="162"/>
-      <c r="F20" s="185"/>
+      <c r="A20" s="176"/>
+      <c r="B20" s="176"/>
+      <c r="C20" s="173"/>
+      <c r="D20" s="176"/>
+      <c r="E20" s="176"/>
+      <c r="F20" s="183"/>
       <c r="G20" s="94" t="s">
         <v>10</v>
       </c>
@@ -8995,17 +8992,17 @@
       <c r="M20" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="O20" s="165"/>
-      <c r="P20" s="165"/>
-      <c r="Q20" s="165"/>
-      <c r="R20" s="165"/>
-      <c r="S20" s="165"/>
+      <c r="O20" s="164"/>
+      <c r="P20" s="164"/>
+      <c r="Q20" s="164"/>
+      <c r="R20" s="164"/>
+      <c r="S20" s="164"/>
       <c r="T20" s="19"/>
-      <c r="V20" s="165"/>
-      <c r="W20" s="165"/>
-      <c r="X20" s="165"/>
-      <c r="Y20" s="165"/>
-      <c r="Z20" s="165"/>
+      <c r="V20" s="164"/>
+      <c r="W20" s="164"/>
+      <c r="X20" s="164"/>
+      <c r="Y20" s="164"/>
+      <c r="Z20" s="164"/>
       <c r="AA20" s="19" t="s">
         <v>20</v>
       </c>
@@ -9026,7 +9023,7 @@
       <c r="D21" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="E21" s="184" t="s">
+      <c r="E21" s="186" t="s">
         <v>104</v>
       </c>
       <c r="F21" s="115">
@@ -9100,7 +9097,7 @@
       <c r="D22" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="E22" s="184"/>
+      <c r="E22" s="186"/>
       <c r="F22" s="115">
         <v>45913</v>
       </c>
@@ -9172,7 +9169,7 @@
       <c r="D23" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="E23" s="184"/>
+      <c r="E23" s="186"/>
       <c r="F23" s="115">
         <v>45910</v>
       </c>
@@ -9244,7 +9241,7 @@
       <c r="D24" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="E24" s="184"/>
+      <c r="E24" s="186"/>
       <c r="F24" s="115">
         <v>45927</v>
       </c>
@@ -9316,7 +9313,7 @@
       <c r="D25" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="E25" s="184"/>
+      <c r="E25" s="186"/>
       <c r="F25" s="115">
         <v>45915</v>
       </c>
@@ -10011,6 +10008,18 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="E21:E25"/>
+    <mergeCell ref="W19:W20"/>
+    <mergeCell ref="K18:K19"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="O18:T18"/>
+    <mergeCell ref="V18:AA18"/>
+    <mergeCell ref="V19:V20"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="D18:D20"/>
+    <mergeCell ref="E18:E20"/>
     <mergeCell ref="AB18:AB19"/>
     <mergeCell ref="F19:F20"/>
     <mergeCell ref="G19:H19"/>
@@ -10024,18 +10033,6 @@
     <mergeCell ref="Q19:Q20"/>
     <mergeCell ref="R19:R20"/>
     <mergeCell ref="S19:S20"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="D18:D20"/>
-    <mergeCell ref="E18:E20"/>
-    <mergeCell ref="E21:E25"/>
-    <mergeCell ref="W19:W20"/>
-    <mergeCell ref="K18:K19"/>
-    <mergeCell ref="M18:M19"/>
-    <mergeCell ref="O18:T18"/>
-    <mergeCell ref="V18:AA18"/>
-    <mergeCell ref="V19:V20"/>
   </mergeCells>
   <conditionalFormatting sqref="C26:C27">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="4DT6">

</xml_diff>